<commit_message>
Updated new cards FAQ
</commit_message>
<xml_diff>
--- a/docs/SVE_FAQ.xlsx
+++ b/docs/SVE_FAQ.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F275"/>
+  <dimension ref="A1:F325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3402,9 +3402,11 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>「変身する」とは、その能力で選んだトークンをゲームから取り除き、取り除いた枚数と同数、別のトークンを同じ領域に作成することを指します。</t>
-        </is>
-      </c>
+          <t>「変身する」とは、その能力で選んだカードをゲームから取り除き、取り除いた枚数と同数、別のトークンを同じ領域に作成することを指します。</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr"/>
+      <c r="F147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -5968,6 +5970,1066 @@
           <t>はい。場のカードの枚数上限より多くカードを場に出す場合、そのスペルや能力をプレイしたプレイヤーが、どのカードを場に出すか選択することができます。</t>
         </is>
       </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="n">
+        <v>275</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>クリスタリアプリンセス・ティア</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>このフォロワー以外の能力で場に出た『クリスタリア・イヴ』は、このフォロワーの能力で目標に選ぶことはできますか？</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>はい。目標に選ぶことができます</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr"/>
+      <c r="F276" t="inlineStr"/>
+    </row>
+    <row r="277">
+      <c r="A277" t="n">
+        <v>276</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>古き森の白狼</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>このフォロワーの《ラストワード》能力でデッキの上から見た4枚の中に《エルフ》フォロワーがあるとき、そのフォロワーを場に出さないことを選ぶことはできますか？</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>はい。場に出さないことを選ぶことができます。</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr"/>
+      <c r="F277" t="inlineStr"/>
+    </row>
+    <row r="278">
+      <c r="A278" t="n">
+        <v>277</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>エルフの少女・リザ</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>このフォロワーが自分の場にあり、相手が『ファイアーチェイン』で2体以上のフォロワーを選んでプレイしたとき、選ばれたフォロワーへのダメージはそれぞれ-1しますか？</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>はい。-1します。</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr"/>
+      <c r="F278" t="inlineStr"/>
+    </row>
+    <row r="279">
+      <c r="A279" t="n">
+        <v>278</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>エルフナイト・シンシア</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>このフォロワーの【攻撃時】能力のコストでEXエリアのカードを消滅するとき、相手のEXエリアのカードを消滅させることはできますか？</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>いいえ。コストは自分の領域のカードやPPなどでしか支払うことができないため、消滅させることはできません。</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr"/>
+      <c r="F279" t="inlineStr"/>
+    </row>
+    <row r="280">
+      <c r="A280" t="n">
+        <v>279</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>エルフの弓術</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>相手の場にフォロワーがないとき、このスペルをプレイすることはできますか？</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>はい。2体まで選ぶとき、0体を選ぶことができるため、プレイすることができます。</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr"/>
+      <c r="F280" t="inlineStr"/>
+    </row>
+    <row r="281">
+      <c r="A281" t="n">
+        <v>280</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>レヴィオンセイバー・アルベール</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>このフォロワーが自分の場に2体あり、それらが攻撃したとき、【攻撃時】能力はそれぞれ1回ずつ誘発しますか？</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>はい。【攻撃時】能力はそれぞれ1ターンに1回ずつ誘発します。</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr"/>
+      <c r="F281" t="inlineStr"/>
+    </row>
+    <row r="282">
+      <c r="A282" t="n">
+        <v>281</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>レヴィオンセイバー・アルベール</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>交戦ダメージとは何ですか？</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>交戦ダメージとは、攻撃フォロワーと攻撃目標のフォロワーが交戦状態のときに、それらのフォロワーが互いに与える攻撃力に等しいダメージのことを指します。</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr"/>
+      <c r="F282" t="inlineStr"/>
+    </row>
+    <row r="283">
+      <c r="A283" t="n">
+        <v>282</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>アレキサンダー</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>このフォロワーが相手のリーダーに攻撃したとき、このフォロワーの「自分のターン中、これが交戦ダメージを与えたとき、これをスタンドする。」能力は誘発しますか？</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>いいえ。攻撃フォロワーが相手のリーダーへ攻撃したときに発生するダメージは交戦ダメージではないため、このフォロワーをスタンドすることはできません。</t>
+        </is>
+      </c>
+      <c r="E283" t="inlineStr"/>
+      <c r="F283" t="inlineStr"/>
+    </row>
+    <row r="284">
+      <c r="A284" t="n">
+        <v>283</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>サムライ</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>このフォロワーの能力で付与された【疾走】と【必殺】は、このフォロワーが場を離れるまで持ち続けますか？</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>はい。持ち続けます。</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr"/>
+      <c r="F284" t="inlineStr"/>
+    </row>
+    <row r="285">
+      <c r="A285" t="n">
+        <v>284</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>次元の魔女・ドロシー</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>このフォロワーが場にあり、自分の墓場のカードが《ウィッチ》フォロワー10枚のみのとき、【スペルチェイン_10】の条件を満たすことはできますか？</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>はい。【スペルチェイン_10】を満たすことができます。</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr"/>
+      <c r="F285" t="inlineStr"/>
+    </row>
+    <row r="286">
+      <c r="A286" t="n">
+        <v>285</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>次元の魔女・ドロシー</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>このフォロワーの《ファンファーレ》能力でEXエリアにカードを置くとき、EXエリアの上限になる前にカードを置くことを止めることはできますか？</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>いいえ。必ずEXエリアの上限になるまでデッキの上からカードを置く必要があります。</t>
+        </is>
+      </c>
+      <c r="E286" t="inlineStr"/>
+      <c r="F286" t="inlineStr"/>
+    </row>
+    <row r="287">
+      <c r="A287" t="n">
+        <v>286</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>次元の魔女・ドロシー</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>このフォロワーの《ファンファーレ》能力でEXエリアにカードを置く際、EXエリアの上限になる前に自分のデッキが0枚になったとき、自分はゲームに敗北しますか？</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>いいえ。デッキが0枚の場合、EXエリアにはカードを置かず、自分はゲームには敗北しません。その後、デッキが0枚で自分がカードを引くとき、自分はゲームに敗北します。</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr"/>
+      <c r="F287" t="inlineStr"/>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>287</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>レヴィオンデューク・ユリウス</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>《Q》とはなんですか？</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>《Q》とは、特定の能力が《Quick》と同様のタイミングでプレイできることを示すアイコンです。
+《Q》を持つ能力は、《Quick》を持つカードと同様に自分のターンのメインフェイズに加え、相手のターンに相手のフォロワーが攻撃してきたときや、相手のエンドフェイズにプレイすることができます。</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr"/>
+      <c r="F288" t="inlineStr"/>
+    </row>
+    <row r="289">
+      <c r="A289" t="n">
+        <v>288</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>レヴィオンデューク・ユリウス</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>《Q》の能力を持つフォロワーやアミュレットは、自分のターンのメインフェイズに加え、相手のターンに相手のフォロワーが攻撃してきたときや、相手のエンドフェイズにプレイし、場に出すことはできますか？</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>いいえ。《Q》は能力が持つアイコンであり、カード自体が《Quick》を持っているわけではないため、フォロワーやアミュレット自体は《Quick》と同様のタイミングではプレイできません。
+《Q》を持つ能力は、その能力がプレイできる領域で《Quick》と同様のタイミングで起動することができます。</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr"/>
+      <c r="F289" t="inlineStr"/>
+    </row>
+    <row r="290">
+      <c r="A290" t="n">
+        <v>289</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>プリンセスマナリア・アン</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>自分の場に『マナリアドラコ・グレア』が2体いるとき、このフォロワーをプレイする際のコストは-4しますか？</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>いいえ。自分の場に『マナリアドラコ・グレア』が2体以上いる場合でも、このフォロワーをプレイする際のコストは-2となります。</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr"/>
+      <c r="F290" t="inlineStr"/>
+    </row>
+    <row r="291">
+      <c r="A291" t="n">
+        <v>290</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>マナリアドラコ・グレア</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>自分の場に『プリンセスマナリア・アン』が2体いるとき、このフォロワーをプレイする際のコストは-4しますか？</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>いいえ。自分の場に『プリンセスマナリア・アン』が2体以上いる場合でも、このフォロワーをプレイする際のコストは-2となります。</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr"/>
+      <c r="F291" t="inlineStr"/>
+    </row>
+    <row r="292">
+      <c r="A292" t="n">
+        <v>291</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>白霜の風</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>このスペルで相手のフォロワーを選ぶ際、【スペルチェイン_10】の条件を満たしているとき、このスペルは相手のエボルヴフォロワーを選ぶことはできますか？</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>いいえ。【スペルチェイン_10】の条件を満たしているかどうかに関わらず、相手の進化していないフォロワーのみを選ぶことができます。</t>
+        </is>
+      </c>
+      <c r="E292" t="inlineStr"/>
+      <c r="F292" t="inlineStr"/>
+    </row>
+    <row r="293">
+      <c r="A293" t="n">
+        <v>292</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>デュアルウィッチ・レミラミ</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>【スタック】を持ち、スタックカウンターが1つ置かれたアミュレット1枚を含めたカードが自分の場に5枚あり、このフォロワーの【進化時】能力をプレイしたとき、『攻撃型ゴーレム』は場に出ますか？</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>はい。能力をプレイするより先にコストが支払われ、かつスタックカウンターが0となったアミュレットが墓場に置かれるため、自分の場は上限ではなくなり『攻撃型ゴーレム』は場に出ます。</t>
+        </is>
+      </c>
+      <c r="E293" t="inlineStr"/>
+      <c r="F293" t="inlineStr"/>
+    </row>
+    <row r="294">
+      <c r="A294" t="n">
+        <v>293</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>連続実験</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>2つ以上の選択肢をチョイスするとき、1つもチョイスしないことを選択することはできますか？</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>いいえ。必ず1つ以上チョイスする必要があります。</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr"/>
+      <c r="F294" t="inlineStr"/>
+    </row>
+    <row r="295">
+      <c r="A295" t="n">
+        <v>294</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>連続実験</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>2つ以上の選択肢をチョイスするとき、１つの選択肢を2回以上チョイスすることはできますか？</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>いいえ。1つの選択肢を2回以上チョイスすることはできません。</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr"/>
+      <c r="F295" t="inlineStr"/>
+    </row>
+    <row r="296">
+      <c r="A296" t="n">
+        <v>295</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>インペリアルドラグーン</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>相手の場にフォロワーがないとき、このフォロワーの《ファンファーレ》能力をプレイせず、手札を捨てないことは選択できますか？</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>いいえ。このフォロワーの《ファンファーレ》能力はコストが無く、プレイしないことを選択できないため、必ず手札を捨てる必要があります。</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr"/>
+      <c r="F296" t="inlineStr"/>
+    </row>
+    <row r="297">
+      <c r="A297" t="n">
+        <v>296</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>竜呼びの笛</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>このアミュレットの《ファンファーレ》能力は、《コスト3》を支払わず、プレイしないことを選択することはできますか？</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>はい。《ファンファーレ》能力のコストを支払わすに、能力をプレイしないことを選択できます。</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr"/>
+      <c r="F297" t="inlineStr"/>
+    </row>
+    <row r="298">
+      <c r="A298" t="n">
+        <v>297</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>竜呼びの笛</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>手札がないとき、このアミュレットの《起動》能力で『ヘルフレイムドラゴン』1枚をEXエリアに置くことはできますか？</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>いいえ。能力のコストを支払うことができないため、『ヘルフレイムドラゴン』をEXエリアに置くことはできません。</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr"/>
+      <c r="F298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" t="n">
+        <v>298</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>竜の闘気</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>自分のPP最大値を+1したとき、自分の残りPPは+1しますか？</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>いいえ。自分の残りPPは+1しません。</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr"/>
+      <c r="F299" t="inlineStr"/>
+    </row>
+    <row r="300">
+      <c r="A300" t="n">
+        <v>299</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>連なる咆哮</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>このアミュレットが自分の場に2枚あり、自分の場に『ドラゴン』が出たとき、このアミュレットの能力はそれぞれ誘発しますか？</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>はい。それぞれ1ターンに1度ずつ能力が誘発します。</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr"/>
+      <c r="F300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" t="n">
+        <v>300</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>ジークフリート</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>このフォロワーの能力は、元々の《体力》の数値が4以上かつ、ダメージなどにより現状の《体力》が3以下のフォロワーを選ぶことができますか？</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>はい。現状の《体力》を参照するため、選ぶことができます。</t>
+        </is>
+      </c>
+      <c r="E301" t="inlineStr"/>
+      <c r="F301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" t="n">
+        <v>301</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>変異の巨竜</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>このフォロワーの能力は、相手のEXエリアのカードを選ぶことはできますか？</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>はい。選ぶことができます。</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr"/>
+      <c r="F302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" t="n">
+        <v>302</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>竜巫女の儀式</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>自分のエンドフェイズに手札の上限枚数となるようにカードを捨てたとき、このアミュレットの「自分のエンドフェイズが来たとき～」の能力はプレイしますか？</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>いいえ。手札の上限枚数となるようにカードを捨てる行為は、「自分のエンドフェイズが来たとき～」の誘発のタイミングよりも後に行うため、条件を満たすことはできず、プレイしません。</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr"/>
+      <c r="F303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" t="n">
+        <v>303</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>ドラゴンテイマー</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>このフォロワーの能力で墓場のカードを選ぶとき、このフォロワーの能力のコストで捨てたカードを選ぶことはできますか？</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>いいえ。コストを支払う前に目標を選ぶ必要があるため、選ぶことはできません。</t>
+        </is>
+      </c>
+      <c r="E304" t="inlineStr"/>
+      <c r="F304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" t="n">
+        <v>304</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>吸血姫・ヴァンピィ</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>このフォロワーが場にあり、新たに『フォレストバット』1体が場に出たとき、このフォロワーは《攻撃力》+1/《体力》+1しますか？</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>いいえ。このフォロワーの《ファンファーレ》能力をプレイしたときに既に場にある『フォレストバット』の数のみを参照するため、新たに『フォレストバット』1体が場に出た場合、このフォロワーは《攻撃力》+1/《体力》+1しません。</t>
+        </is>
+      </c>
+      <c r="E305" t="inlineStr"/>
+      <c r="F305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" t="n">
+        <v>305</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>ラプラスの魔 ラプラス・ダークネス</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>カードの名前が2つありますが、これは何ですか？</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>名前が2つあるカードには、カード名とコラボ名が存在します。
+名前が2つあるカードはルール上、上側に書かれたカード名のカードとして扱います。
+特定のカード名を参照するカードや能力をプレイする際、これらのカードは上側に書かれたカード名を参照します。</t>
+        </is>
+      </c>
+      <c r="E306" t="inlineStr"/>
+      <c r="F306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" t="n">
+        <v>306</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>ソウルディーラー</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>このフォロワーの【進化時】能力で破壊した相手のフォロワーの《攻撃力》が増減していたとき、Xは増減後の《攻撃力》の数値ですか？</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>はい。その通りです。</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr"/>
+      <c r="F307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" t="n">
+        <v>307</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>冥守の戦士・カムラ</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>このフォロワーの《ラストワード》能力で破壊した相手のフォロワーの《攻撃力》が増減していたとき、Xは増減後の《攻撃力》の数値ですか？</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>はい。その通りです。</t>
+        </is>
+      </c>
+      <c r="E308" t="inlineStr"/>
+      <c r="F308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="n">
+        <v>308</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>アザゼル</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>プレイヤーが自身のカードを捨てるとき、どのような方法で捨てるカードをランダムに選択しますか？</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>ダイスロールなど、無作為な方法で選択します。</t>
+        </is>
+      </c>
+      <c r="E309" t="inlineStr"/>
+      <c r="F309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" t="n">
+        <v>309</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>アザゼル</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>相手のリーダーの《体力》が9以下のとき、このフォロワーの【進化時】能力で相手の《体力》は10になりますか？</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>はい。10になります。</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr"/>
+      <c r="F310" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" t="n">
+        <v>312</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>享楽の悪魔</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>このフォロワーの【攻撃時】能力は、自分のリーダーにも1ダメージを与えますか？</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>はい。自分のリーダーにも1ダメージを与えます。</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr"/>
+      <c r="F313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" t="n">
+        <v>313</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>ボーンキマイラ</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>このフォロワーの【ネクロチャージ_7】の条件を満たしている状態で墓場のカードが移動し、墓場のカードが6枚以下になったとき、このフォロワーの【突進】と【必殺】は失われますか？</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>はい。失われます。</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr"/>
+      <c r="F314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" t="n">
+        <v>314</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>ヘヴンリーイージス</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>このフォロワーが進化するとき、「《コスト2》」と「手札3枚を捨てる」両方を支払う必要がありますか？</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>いいえ。このフォロワーが進化するとき、「《コスト2》」と「手札3枚を捨てる」はどちらかを支払えば進化することができます。</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr"/>
+      <c r="F315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" t="n">
+        <v>315</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>ヘヴンリーイージス</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>『夢兎の白兎』の「《起動》《コスト10》これを《アクト》墓場に置く：フォロワーすべてを消滅させる。」で、このフォロワーは消滅しますか？</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>はい。消滅します。</t>
+        </is>
+      </c>
+      <c r="E316" t="inlineStr"/>
+      <c r="F316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="n">
+        <v>316</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>封じられし熾天使</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>『ダークオファリング』で自分の場のこのアミュレットを選んだとき、効果でこのアミュレットは破壊されますか？</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>いいえ。破壊されません。</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr"/>
+      <c r="F317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" t="n">
+        <v>317</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>カグヤ</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>このフォロワーが自分の場にあり、アミュレットが2枚同時に自分の場に出たとき、このフォロワーの「自分の場にアミュレットが出たとき～」の能力は2回誘発しますか？</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>はい。場に出たアミュレットの数と同数回誘発します。</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr"/>
+      <c r="F318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>318</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>エイラの祈祷</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>このアミュレットが自分の場に2枚あり、自分のリーダーの《体力》を＋したとき、このアミュレットの能力はそれぞれ誘発しますか？</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>はい。それぞれ1ターンに1度ずつ能力が誘発します。</t>
+        </is>
+      </c>
+      <c r="E319" t="inlineStr"/>
+      <c r="F319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" t="n">
+        <v>319</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>サファイアプリースト</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>自分のフォロワーが攻撃し、その攻撃フォロワーが《Quick》を持つカードや能力によって場を離れたとき、その攻撃はこのフォロワーの能力の条件に数えることはできますか？</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>はい。攻撃している間にその攻撃フォロワーが場を離れても、その攻撃を数えることができます。</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr"/>
+      <c r="F320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" t="n">
+        <v>320</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>スレッジエクソシスト</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>このフォロワーの《ファンファーレ》能力は、《コスト2》を支払わず、プレイしないことを選択することはできますか？</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>はい。《ファンファーレ》能力のコストを支払わすに、能力をプレイしないことを選択できます。</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr"/>
+      <c r="F321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" t="n">
+        <v>321</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>エメラルドメイデン</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>このフォロワーの《ファンファーレ》能力で【守護】を持つ自分のフォロワーを数えるとき、このフォロワーを数えることはできますか？</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>いいえ。このフォロワー以外の【守護】を持つフォロワーのみを数えます。</t>
+        </is>
+      </c>
+      <c r="E322" t="inlineStr"/>
+      <c r="F322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" t="n">
+        <v>322</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>アークエンジェル・レイナ</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>このフォロワーの【進化時】能力で裏向きにしたエボルヴデッキのエボルヴフォロワーは、《進化》で再度使用することはできますか？</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>はい。表向きから裏向きにしたエボルヴデッキのエボルヴフォロワーは、《進化》で再度使用することができます。</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr"/>
+      <c r="F323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" t="n">
+        <v>323</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>氷獄の呼び声</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>相手の場にフォロワーがないとき、このスペルをプレイし自分のデッキからニュートラルフォロワーを探して手札に加えることはできますか？</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>いいえ。相手の場にいるフォロワーを選ぶことができないため、このスペルをプレイすることはできません。</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr"/>
+      <c r="F324" t="inlineStr"/>
+    </row>
+    <row r="325">
+      <c r="A325" t="n">
+        <v>324</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>ドラゴウェポン</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>タイプを持つとは何ですか？</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>タイプを持つとは、そのカードが持つ元々のタイプに加え、効果によって新たにタイプが追加されることを示します。</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr"/>
+      <c r="F325" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated Card Name Translation for FAQ
</commit_message>
<xml_diff>
--- a/docs/SVE_FAQ.xlsx
+++ b/docs/SVE_FAQ.xlsx
@@ -3405,8 +3405,6 @@
           <t>「変身する」とは、その能力で選んだカードをゲームから取り除き、取り除いた枚数と同数、別のトークンを同じ領域に作成することを指します。</t>
         </is>
       </c>
-      <c r="E147" t="inlineStr"/>
-      <c r="F147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -5990,8 +5988,6 @@
           <t>はい。目標に選ぶことができます</t>
         </is>
       </c>
-      <c r="E276" t="inlineStr"/>
-      <c r="F276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" t="n">
@@ -6012,8 +6008,6 @@
           <t>はい。場に出さないことを選ぶことができます。</t>
         </is>
       </c>
-      <c r="E277" t="inlineStr"/>
-      <c r="F277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" t="n">
@@ -6034,8 +6028,6 @@
           <t>はい。-1します。</t>
         </is>
       </c>
-      <c r="E278" t="inlineStr"/>
-      <c r="F278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" t="n">
@@ -6056,8 +6048,6 @@
           <t>いいえ。コストは自分の領域のカードやPPなどでしか支払うことができないため、消滅させることはできません。</t>
         </is>
       </c>
-      <c r="E279" t="inlineStr"/>
-      <c r="F279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="n">
@@ -6078,8 +6068,6 @@
           <t>はい。2体まで選ぶとき、0体を選ぶことができるため、プレイすることができます。</t>
         </is>
       </c>
-      <c r="E280" t="inlineStr"/>
-      <c r="F280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" t="n">
@@ -6100,8 +6088,6 @@
           <t>はい。【攻撃時】能力はそれぞれ1ターンに1回ずつ誘発します。</t>
         </is>
       </c>
-      <c r="E281" t="inlineStr"/>
-      <c r="F281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" t="n">
@@ -6122,8 +6108,6 @@
           <t>交戦ダメージとは、攻撃フォロワーと攻撃目標のフォロワーが交戦状態のときに、それらのフォロワーが互いに与える攻撃力に等しいダメージのことを指します。</t>
         </is>
       </c>
-      <c r="E282" t="inlineStr"/>
-      <c r="F282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" t="n">
@@ -6144,8 +6128,6 @@
           <t>いいえ。攻撃フォロワーが相手のリーダーへ攻撃したときに発生するダメージは交戦ダメージではないため、このフォロワーをスタンドすることはできません。</t>
         </is>
       </c>
-      <c r="E283" t="inlineStr"/>
-      <c r="F283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" t="n">
@@ -6166,8 +6148,6 @@
           <t>はい。持ち続けます。</t>
         </is>
       </c>
-      <c r="E284" t="inlineStr"/>
-      <c r="F284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" t="n">
@@ -6188,8 +6168,6 @@
           <t>はい。【スペルチェイン_10】を満たすことができます。</t>
         </is>
       </c>
-      <c r="E285" t="inlineStr"/>
-      <c r="F285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" t="n">
@@ -6210,8 +6188,6 @@
           <t>いいえ。必ずEXエリアの上限になるまでデッキの上からカードを置く必要があります。</t>
         </is>
       </c>
-      <c r="E286" t="inlineStr"/>
-      <c r="F286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" t="n">
@@ -6232,8 +6208,6 @@
           <t>いいえ。デッキが0枚の場合、EXエリアにはカードを置かず、自分はゲームには敗北しません。その後、デッキが0枚で自分がカードを引くとき、自分はゲームに敗北します。</t>
         </is>
       </c>
-      <c r="E287" t="inlineStr"/>
-      <c r="F287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="n">
@@ -6255,8 +6229,6 @@
 《Q》を持つ能力は、《Quick》を持つカードと同様に自分のターンのメインフェイズに加え、相手のターンに相手のフォロワーが攻撃してきたときや、相手のエンドフェイズにプレイすることができます。</t>
         </is>
       </c>
-      <c r="E288" t="inlineStr"/>
-      <c r="F288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="n">
@@ -6278,8 +6250,6 @@
 《Q》を持つ能力は、その能力がプレイできる領域で《Quick》と同様のタイミングで起動することができます。</t>
         </is>
       </c>
-      <c r="E289" t="inlineStr"/>
-      <c r="F289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" t="n">
@@ -6300,8 +6270,6 @@
           <t>いいえ。自分の場に『マナリアドラコ・グレア』が2体以上いる場合でも、このフォロワーをプレイする際のコストは-2となります。</t>
         </is>
       </c>
-      <c r="E290" t="inlineStr"/>
-      <c r="F290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" t="n">
@@ -6322,8 +6290,6 @@
           <t>いいえ。自分の場に『プリンセスマナリア・アン』が2体以上いる場合でも、このフォロワーをプレイする際のコストは-2となります。</t>
         </is>
       </c>
-      <c r="E291" t="inlineStr"/>
-      <c r="F291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" t="n">
@@ -6344,8 +6310,6 @@
           <t>いいえ。【スペルチェイン_10】の条件を満たしているかどうかに関わらず、相手の進化していないフォロワーのみを選ぶことができます。</t>
         </is>
       </c>
-      <c r="E292" t="inlineStr"/>
-      <c r="F292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" t="n">
@@ -6366,8 +6330,6 @@
           <t>はい。能力をプレイするより先にコストが支払われ、かつスタックカウンターが0となったアミュレットが墓場に置かれるため、自分の場は上限ではなくなり『攻撃型ゴーレム』は場に出ます。</t>
         </is>
       </c>
-      <c r="E293" t="inlineStr"/>
-      <c r="F293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" t="n">
@@ -6388,8 +6350,6 @@
           <t>いいえ。必ず1つ以上チョイスする必要があります。</t>
         </is>
       </c>
-      <c r="E294" t="inlineStr"/>
-      <c r="F294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" t="n">
@@ -6410,8 +6370,6 @@
           <t>いいえ。1つの選択肢を2回以上チョイスすることはできません。</t>
         </is>
       </c>
-      <c r="E295" t="inlineStr"/>
-      <c r="F295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" t="n">
@@ -6432,8 +6390,6 @@
           <t>いいえ。このフォロワーの《ファンファーレ》能力はコストが無く、プレイしないことを選択できないため、必ず手札を捨てる必要があります。</t>
         </is>
       </c>
-      <c r="E296" t="inlineStr"/>
-      <c r="F296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" t="n">
@@ -6454,8 +6410,6 @@
           <t>はい。《ファンファーレ》能力のコストを支払わすに、能力をプレイしないことを選択できます。</t>
         </is>
       </c>
-      <c r="E297" t="inlineStr"/>
-      <c r="F297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" t="n">
@@ -6476,8 +6430,6 @@
           <t>いいえ。能力のコストを支払うことができないため、『ヘルフレイムドラゴン』をEXエリアに置くことはできません。</t>
         </is>
       </c>
-      <c r="E298" t="inlineStr"/>
-      <c r="F298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" t="n">
@@ -6498,8 +6450,6 @@
           <t>いいえ。自分の残りPPは+1しません。</t>
         </is>
       </c>
-      <c r="E299" t="inlineStr"/>
-      <c r="F299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" t="n">
@@ -6520,8 +6470,6 @@
           <t>はい。それぞれ1ターンに1度ずつ能力が誘発します。</t>
         </is>
       </c>
-      <c r="E300" t="inlineStr"/>
-      <c r="F300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" t="n">
@@ -6542,8 +6490,6 @@
           <t>はい。現状の《体力》を参照するため、選ぶことができます。</t>
         </is>
       </c>
-      <c r="E301" t="inlineStr"/>
-      <c r="F301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" t="n">
@@ -6564,8 +6510,6 @@
           <t>はい。選ぶことができます。</t>
         </is>
       </c>
-      <c r="E302" t="inlineStr"/>
-      <c r="F302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" t="n">
@@ -6586,8 +6530,6 @@
           <t>いいえ。手札の上限枚数となるようにカードを捨てる行為は、「自分のエンドフェイズが来たとき～」の誘発のタイミングよりも後に行うため、条件を満たすことはできず、プレイしません。</t>
         </is>
       </c>
-      <c r="E303" t="inlineStr"/>
-      <c r="F303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" t="n">
@@ -6608,8 +6550,6 @@
           <t>いいえ。コストを支払う前に目標を選ぶ必要があるため、選ぶことはできません。</t>
         </is>
       </c>
-      <c r="E304" t="inlineStr"/>
-      <c r="F304" t="inlineStr"/>
     </row>
     <row r="305">
       <c r="A305" t="n">
@@ -6630,8 +6570,6 @@
           <t>いいえ。このフォロワーの《ファンファーレ》能力をプレイしたときに既に場にある『フォレストバット』の数のみを参照するため、新たに『フォレストバット』1体が場に出た場合、このフォロワーは《攻撃力》+1/《体力》+1しません。</t>
         </is>
       </c>
-      <c r="E305" t="inlineStr"/>
-      <c r="F305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" t="n">
@@ -6654,8 +6592,6 @@
 特定のカード名を参照するカードや能力をプレイする際、これらのカードは上側に書かれたカード名を参照します。</t>
         </is>
       </c>
-      <c r="E306" t="inlineStr"/>
-      <c r="F306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" t="n">
@@ -6676,8 +6612,6 @@
           <t>はい。その通りです。</t>
         </is>
       </c>
-      <c r="E307" t="inlineStr"/>
-      <c r="F307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" t="n">
@@ -6698,8 +6632,6 @@
           <t>はい。その通りです。</t>
         </is>
       </c>
-      <c r="E308" t="inlineStr"/>
-      <c r="F308" t="inlineStr"/>
     </row>
     <row r="309">
       <c r="A309" t="n">
@@ -6720,8 +6652,6 @@
           <t>ダイスロールなど、無作為な方法で選択します。</t>
         </is>
       </c>
-      <c r="E309" t="inlineStr"/>
-      <c r="F309" t="inlineStr"/>
     </row>
     <row r="310">
       <c r="A310" t="n">
@@ -6742,8 +6672,6 @@
           <t>はい。10になります。</t>
         </is>
       </c>
-      <c r="E310" t="inlineStr"/>
-      <c r="F310" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" t="n">
@@ -6764,8 +6692,6 @@
           <t>はい。自分のリーダーにも1ダメージを与えます。</t>
         </is>
       </c>
-      <c r="E313" t="inlineStr"/>
-      <c r="F313" t="inlineStr"/>
     </row>
     <row r="314">
       <c r="A314" t="n">
@@ -6786,8 +6712,6 @@
           <t>はい。失われます。</t>
         </is>
       </c>
-      <c r="E314" t="inlineStr"/>
-      <c r="F314" t="inlineStr"/>
     </row>
     <row r="315">
       <c r="A315" t="n">
@@ -6808,8 +6732,6 @@
           <t>いいえ。このフォロワーが進化するとき、「《コスト2》」と「手札3枚を捨てる」はどちらかを支払えば進化することができます。</t>
         </is>
       </c>
-      <c r="E315" t="inlineStr"/>
-      <c r="F315" t="inlineStr"/>
     </row>
     <row r="316">
       <c r="A316" t="n">
@@ -6830,8 +6752,6 @@
           <t>はい。消滅します。</t>
         </is>
       </c>
-      <c r="E316" t="inlineStr"/>
-      <c r="F316" t="inlineStr"/>
     </row>
     <row r="317">
       <c r="A317" t="n">
@@ -6852,8 +6772,6 @@
           <t>いいえ。破壊されません。</t>
         </is>
       </c>
-      <c r="E317" t="inlineStr"/>
-      <c r="F317" t="inlineStr"/>
     </row>
     <row r="318">
       <c r="A318" t="n">
@@ -6874,8 +6792,6 @@
           <t>はい。場に出たアミュレットの数と同数回誘発します。</t>
         </is>
       </c>
-      <c r="E318" t="inlineStr"/>
-      <c r="F318" t="inlineStr"/>
     </row>
     <row r="319">
       <c r="A319" t="n">
@@ -6896,8 +6812,6 @@
           <t>はい。それぞれ1ターンに1度ずつ能力が誘発します。</t>
         </is>
       </c>
-      <c r="E319" t="inlineStr"/>
-      <c r="F319" t="inlineStr"/>
     </row>
     <row r="320">
       <c r="A320" t="n">
@@ -6918,8 +6832,6 @@
           <t>はい。攻撃している間にその攻撃フォロワーが場を離れても、その攻撃を数えることができます。</t>
         </is>
       </c>
-      <c r="E320" t="inlineStr"/>
-      <c r="F320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" t="n">
@@ -6940,8 +6852,6 @@
           <t>はい。《ファンファーレ》能力のコストを支払わすに、能力をプレイしないことを選択できます。</t>
         </is>
       </c>
-      <c r="E321" t="inlineStr"/>
-      <c r="F321" t="inlineStr"/>
     </row>
     <row r="322">
       <c r="A322" t="n">
@@ -6962,8 +6872,6 @@
           <t>いいえ。このフォロワー以外の【守護】を持つフォロワーのみを数えます。</t>
         </is>
       </c>
-      <c r="E322" t="inlineStr"/>
-      <c r="F322" t="inlineStr"/>
     </row>
     <row r="323">
       <c r="A323" t="n">
@@ -6984,8 +6892,6 @@
           <t>はい。表向きから裏向きにしたエボルヴデッキのエボルヴフォロワーは、《進化》で再度使用することができます。</t>
         </is>
       </c>
-      <c r="E323" t="inlineStr"/>
-      <c r="F323" t="inlineStr"/>
     </row>
     <row r="324">
       <c r="A324" t="n">
@@ -7006,8 +6912,6 @@
           <t>いいえ。相手の場にいるフォロワーを選ぶことができないため、このスペルをプレイすることはできません。</t>
         </is>
       </c>
-      <c r="E324" t="inlineStr"/>
-      <c r="F324" t="inlineStr"/>
     </row>
     <row r="325">
       <c r="A325" t="n">
@@ -7028,8 +6932,6 @@
           <t>タイプを持つとは、そのカードが持つ元々のタイプに加え、効果によって新たにタイプが追加されることを示します。</t>
         </is>
       </c>
-      <c r="E325" t="inlineStr"/>
-      <c r="F325" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated promo cards and FAQ
</commit_message>
<xml_diff>
--- a/docs/SVE_FAQ.xlsx
+++ b/docs/SVE_FAQ.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F325"/>
+  <dimension ref="A1:F338"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6933,6 +6933,313 @@
         </is>
       </c>
     </row>
+    <row r="326">
+      <c r="A326" t="n">
+        <v>325</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>キーワード</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>【指定攻撃】を持つフォロワーは、相手の【守護】を持つアクト状態のフォロワーを無視して相手の他のフォロワーに攻撃できますか？</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>いいえ。必ずアクト状態の【守護】を持つフォロワーを選ぶ必要があります。</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr"/>
+      <c r="F326" t="inlineStr"/>
+    </row>
+    <row r="327">
+      <c r="A327" t="n">
+        <v>326</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>アーチャー</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>『エンシェントエルフ』の《ファンファーレ》能力のコストで『アーチャー』を選択した場合、『アーチャー』の能力はプレイしますか？</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>はい。一度誘発した自動能力は、そのカードが場を離れても能力をプレイできます。</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr"/>
+      <c r="F327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" t="n">
+        <v>327</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>クラフトウォーロック</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>『クラフトウォーロック(EVOLVE)』の能力で「【スタック】+1する」は自分の【スタック】を持つアミュレット全ての【スタック】を+できますか？</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">いいえ。【スタック】を持つアミュレット1枚を選択し、そのカードのスタックカウンターを+1します。
+</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr"/>
+      <c r="F328" t="inlineStr"/>
+    </row>
+    <row r="329">
+      <c r="A329" t="n">
+        <v>328</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>キーワード</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">【スタック】を持つアミュレットを『エクスキューション』で破壊した場合、【スタック】能力でスタックカウンターを取り除くことで、場に残せますか？
+</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">はい。自分や相手のカード問わず、場を離れる時に【スタック】能力でスタックカウンターを取り除くことで場に残せます。
+</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr"/>
+      <c r="F329" t="inlineStr"/>
+    </row>
+    <row r="330">
+      <c r="A330" t="n">
+        <v>329</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>次元の魔女・ドロシー</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">『次元の魔女・ドロシー(EVOLVE)』の【進化時】能力でコストが-5された『次元の超越』をプレイする際、さらに『次元の超越』の能力でコストを7にする場合、コストは7から-5をし、コスト2でプレイできますか？
+</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">はい。コスト2でプレイすることができます。
+</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr"/>
+      <c r="F330" t="inlineStr"/>
+    </row>
+    <row r="331">
+      <c r="A331" t="n">
+        <v>330</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>キーワード</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">【進化時】能力が複数あるカードに進化した場合、その能力は全てプレイしますか？
+</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">はい。【進化時】能力が複数ある場合でも、全てプレイします。
+</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr"/>
+      <c r="F331" t="inlineStr"/>
+    </row>
+    <row r="332">
+      <c r="A332" t="n">
+        <v>331</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>裁きの悪魔</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">このフォロワーが相手のフォロワーと交戦した際に、お互いのフォロワーが破壊された場合、このフォロワーの能力はプレイできますか？
+</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">はい。交戦でお互いが破壊された場合でも「破壊されたとき」を満たしているため、プレイすることができます。
+</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr"/>
+      <c r="F332" t="inlineStr"/>
+    </row>
+    <row r="333">
+      <c r="A333" t="n">
+        <v>332</v>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>享楽の悪魔</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">このフォロワーの能力は、【真紅】状態でない場合でも手札を1枚捨てますか？
+</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">いいえ。「【真紅】状態なら」の以降の能力は、条件を満たさない場合、プレイできません。
+</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr"/>
+      <c r="F333" t="inlineStr"/>
+    </row>
+    <row r="334">
+      <c r="A334" t="n">
+        <v>333</v>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>エイラの祈祷</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">このアミュレットの能力は相手のターンでもプレイできますか？
+</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">はい。相手のターンでも条件を満たせば、能力はプレイできます。
+</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr"/>
+      <c r="F334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" t="n">
+        <v>334</v>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>神域の守護者</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">このアミュレットの能力は相手のターンでもプレイできますか？
+</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">いいえ。このアミュレットの能力は自分のターンのみプレイできます。
+</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr"/>
+      <c r="F335" t="inlineStr"/>
+    </row>
+    <row r="336">
+      <c r="A336" t="n">
+        <v>335</v>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>エイラの祈祷</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">『ダークオファリング』の能力で『エイラの祈祷』を選択し、そのカードを破壊して、リーダーの《体力》を+した場合、『エイラの祈祷』の能力はプレイできますか？
+</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">いいえ。『ダークオファリング』で自分のリーダーを《体力》+3したとき、『エイラの祈祷』が場にないため「リーダーの《体力》を+したとき」の能力はプレイできません。
+</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr"/>
+      <c r="F336" t="inlineStr"/>
+    </row>
+    <row r="337">
+      <c r="A337" t="n">
+        <v>336</v>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>ダークエンジェル・オリヴィエ</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">先攻のプレイヤーが『ダークエンジェル・オリヴィエ』の能力でEPを+1できますか？
+</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">はい。先攻後攻問わず、全てのプレイヤーは能力でEPを得ます。
+</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr"/>
+      <c r="F337" t="inlineStr"/>
+    </row>
+    <row r="338">
+      <c r="A338" t="n">
+        <v>337</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>ダークエンジェル・オリヴィエ</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EPが3ある状態で『ダークエンジェル・オリヴィエ』の能力でEPを+1できますか？
+</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">はい。EPは上限がないため、EPが3ある場合も新たにEPを得ます。
+</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr"/>
+      <c r="F338" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>